<commit_message>
update mcu io map
</commit_message>
<xml_diff>
--- a/Carrot-Inside-STM32H743XIH6-Board.Ver.A/Pinout_Ver.A.xlsx
+++ b/Carrot-Inside-STM32H743XIH6-Board.Ver.A/Pinout_Ver.A.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yummycarrot\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Carrot-Inside-STM32-Board\Carrot-Inside-STM32H743XIH6-Board.Ver.A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1521C9F-A1D6-4CF7-BA03-CEFF3FFE1163}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBA3106-9D7C-4EE1-9BED-C5691A83D656}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -748,7 +748,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -928,8 +928,44 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1044,6 +1080,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1173,8 +1224,29 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1534,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1545,684 +1617,684 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+      <c r="A23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+      <c r="A25" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+      <c r="A26" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
+      <c r="A27" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
+      <c r="A28" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="5" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+      <c r="A30" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+      <c r="A31" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+      <c r="A32" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="A33" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="6" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+      <c r="A34" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="6" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+      <c r="A35" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="6" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
+      <c r="A36" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="6" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
+      <c r="A37" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="6" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
+      <c r="A38" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="6" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
+      <c r="A39" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
+      <c r="A40" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
+      <c r="A41" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+      <c r="A42" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="7" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
+      <c r="A43" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
+      <c r="A44" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
+      <c r="A45" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="7" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
+      <c r="A46" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="7" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
+      <c r="A47" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
+      <c r="A48" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
+      <c r="A49" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
+      <c r="A50" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
+      <c r="A58" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
+      <c r="A59" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
+      <c r="A60" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
+      <c r="A61" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
+      <c r="A62" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="3" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>